<commit_message>
first step modification changes
</commit_message>
<xml_diff>
--- a/QR_TestData.xlsx
+++ b/QR_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12915" windowHeight="5850"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12390" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="QR_TestData" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="263">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -809,6 +809,9 @@
   </si>
   <si>
     <t>Transfer_04</t>
+  </si>
+  <si>
+    <t>9000000003</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1232,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1239,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1286,7 +1289,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>204</v>
+        <v>262</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -1331,7 +1334,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>204</v>
+        <v>262</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
@@ -1345,7 +1348,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>204</v>
+        <v>262</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>

</xml_diff>